<commit_message>
Fix for InfoMapper updates, issue #31
Fixed favicon, polygon render order.
Also cleaned up boating data.
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Recreation-BoatingOrganizations/data/boating-orgs-data.xlsx
+++ b/workflow/BasinEntities/Recreation-BoatingOrganizations/data/boating-orgs-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Organization</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Whitewater river conservation</t>
   </si>
   <si>
-    <t>americanwhitewater.org</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -121,6 +118,12 @@
   </si>
   <si>
     <t>Mountain Whitewater</t>
+  </si>
+  <si>
+    <t>https://www.fcgov.com/parkplanning/poudre-river-park</t>
+  </si>
+  <si>
+    <t>https://www.americanwhitewater.org/</t>
   </si>
 </sst>
 </file>
@@ -469,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,10 +516,10 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -556,10 +559,10 @@
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
         <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
       </c>
       <c r="G3">
         <v>-104.575237</v>
@@ -576,18 +579,20 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
@@ -623,7 +628,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -649,8 +654,10 @@
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E6" r:id="rId2"/>
     <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add links to info pages pointing to app resources, issue #135
Also enabled local food entities layer.
Cleaned up snowpack maps.
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Recreation-BoatingOrganizations/data/boating-orgs-data.xlsx
+++ b/workflow/BasinEntities/Recreation-BoatingOrganizations/data/boating-orgs-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Organization</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>https://www.americanwhitewater.org/</t>
+  </si>
+  <si>
+    <t>Poudre Paddlers</t>
+  </si>
+  <si>
+    <t>https://www.poudrepaddlers.org/</t>
+  </si>
+  <si>
+    <t>Canoe and kayak club</t>
   </si>
 </sst>
 </file>
@@ -470,10 +479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,82 +588,105 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4">
-        <v>-105.075684</v>
+        <v>-105.08152</v>
       </c>
       <c r="H4">
-        <v>40.595204000000003</v>
+        <v>40.583629999999999</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
       <c r="G5">
-        <v>-105.096104</v>
+        <v>-105.075684</v>
       </c>
       <c r="H5">
-        <v>40.625228999999997</v>
+        <v>40.595204000000003</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
       <c r="G6">
+        <v>-105.096104</v>
+      </c>
+      <c r="H6">
+        <v>40.625228999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7">
         <v>-105.101062</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>40.625219000000001</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E6" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
     <hyperlink ref="E3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>